<commit_message>
rough schematic and component requirement defenition
</commit_message>
<xml_diff>
--- a/documentation/rough-budget.xlsx
+++ b/documentation/rough-budget.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Component</t>
   </si>
@@ -125,6 +125,30 @@
   </si>
   <si>
     <t>Mouser | Digikey</t>
+  </si>
+  <si>
+    <t>Sense Resistor</t>
+  </si>
+  <si>
+    <t>WSLF25121L000FEA</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>1mΩ 6W</t>
+  </si>
+  <si>
+    <t>Current Amplifier</t>
+  </si>
+  <si>
+    <t>AD8418</t>
+  </si>
+  <si>
+    <t>Analog Devices</t>
+  </si>
+  <si>
+    <t>Bidirectional, Zero Drift, Current Sense Amplifier High accuracy gain = 20</t>
   </si>
   <si>
     <t>PCB</t>
@@ -147,11 +171,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="#,##0.00&quot;€&quot;;\-#,##0.00&quot;€&quot;"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -169,14 +193,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Georgia"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Georgia"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Georgia"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Georgia"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Georgia"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Georgia"/>
@@ -192,34 +247,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Georgia"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Georgia"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Georgia"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Georgia"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -230,18 +262,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Georgia"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Georgia"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -261,15 +286,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Georgia"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Georgia"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -282,25 +299,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Georgia"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Georgia"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="Georgia"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,6 +320,22 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Georgia"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Georgia"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -340,187 +364,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,17 +717,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,21 +777,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -765,28 +794,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -795,152 +819,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -972,12 +996,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -1325,7 +1343,7 @@
   <dimension ref="B1:K32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1369,7 +1387,7 @@
       <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1391,13 +1409,13 @@
       <c r="H3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="13">
         <v>1</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="14">
         <v>12.87</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="15">
         <f>J3*I3</f>
         <v>12.87</v>
       </c>
@@ -1420,13 +1438,13 @@
       <c r="H4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="16">
         <v>4</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="17">
         <v>3.05</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="15">
         <f t="shared" ref="K4:K14" si="0">J4*I4</f>
         <v>12.2</v>
       </c>
@@ -1451,13 +1469,13 @@
       <c r="H5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="16">
         <v>8</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="17">
         <v>1.6</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="15">
         <f t="shared" si="0"/>
         <v>12.8</v>
       </c>
@@ -1480,13 +1498,13 @@
       <c r="H6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="16">
         <v>1</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="17">
         <v>1.89</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="15">
         <f t="shared" si="0"/>
         <v>1.89</v>
       </c>
@@ -1508,16 +1526,16 @@
       <c r="G7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <v>1</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="17">
         <v>45.46</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="15">
         <f t="shared" si="0"/>
         <v>45.46</v>
       </c>
@@ -1542,13 +1560,13 @@
       <c r="H8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="16">
         <v>1</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="17">
         <v>20</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="15">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1570,56 +1588,80 @@
       <c r="G9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="18">
+      <c r="H9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="16">
+        <v>2</v>
+      </c>
+      <c r="J9" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="15">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J9" s="19">
+    </row>
+    <row r="10" ht="15.75" spans="2:11">
+      <c r="B10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="16">
+        <v>2</v>
+      </c>
+      <c r="J10" s="17">
+        <v>2.5</v>
+      </c>
+      <c r="K10" s="15">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" spans="2:11">
+      <c r="B11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="16">
+        <v>1</v>
+      </c>
+      <c r="J11" s="17">
         <v>10</v>
       </c>
-      <c r="K9" s="17">
-        <f t="shared" si="0"/>
+      <c r="K11" s="15">
+        <f>J11*I11</f>
         <v>10</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" spans="2:11">
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="18">
-        <v>0</v>
-      </c>
-      <c r="J10" s="19">
-        <v>0</v>
-      </c>
-      <c r="K10" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" spans="2:11">
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="18">
-        <v>0</v>
-      </c>
-      <c r="J11" s="19">
-        <v>0</v>
-      </c>
-      <c r="K11" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="2:11">
@@ -1629,14 +1671,14 @@
       <c r="E12" s="6"/>
       <c r="F12" s="10"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="18">
-        <v>0</v>
-      </c>
-      <c r="J12" s="19">
-        <v>0</v>
-      </c>
-      <c r="K12" s="17">
+      <c r="H12" s="10"/>
+      <c r="I12" s="16">
+        <v>0</v>
+      </c>
+      <c r="J12" s="17">
+        <v>0</v>
+      </c>
+      <c r="K12" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1648,14 +1690,14 @@
       <c r="E13" s="6"/>
       <c r="F13" s="10"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="18">
-        <v>0</v>
-      </c>
-      <c r="J13" s="19">
-        <v>0</v>
-      </c>
-      <c r="K13" s="17">
+      <c r="H13" s="10"/>
+      <c r="I13" s="16">
+        <v>0</v>
+      </c>
+      <c r="J13" s="17">
+        <v>0</v>
+      </c>
+      <c r="K13" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1667,14 +1709,14 @@
       <c r="E14" s="6"/>
       <c r="F14" s="10"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="18">
-        <v>0</v>
-      </c>
-      <c r="J14" s="19">
-        <v>0</v>
-      </c>
-      <c r="K14" s="17">
+      <c r="H14" s="10"/>
+      <c r="I14" s="16">
+        <v>0</v>
+      </c>
+      <c r="J14" s="17">
+        <v>0</v>
+      </c>
+      <c r="K14" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1686,14 +1728,14 @@
       <c r="E15" s="6"/>
       <c r="F15" s="10"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="18">
-        <v>0</v>
-      </c>
-      <c r="J15" s="19">
-        <v>0</v>
-      </c>
-      <c r="K15" s="17">
+      <c r="H15" s="10"/>
+      <c r="I15" s="16">
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
+        <v>0</v>
+      </c>
+      <c r="K15" s="15">
         <f t="shared" ref="K15:K30" si="1">J15*I15</f>
         <v>0</v>
       </c>
@@ -1705,14 +1747,14 @@
       <c r="E16" s="6"/>
       <c r="F16" s="10"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="18">
-        <v>0</v>
-      </c>
-      <c r="J16" s="19">
-        <v>0</v>
-      </c>
-      <c r="K16" s="17">
+      <c r="H16" s="10"/>
+      <c r="I16" s="16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="17">
+        <v>0</v>
+      </c>
+      <c r="K16" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1724,14 +1766,14 @@
       <c r="E17" s="6"/>
       <c r="F17" s="10"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="18">
-        <v>0</v>
-      </c>
-      <c r="J17" s="19">
-        <v>0</v>
-      </c>
-      <c r="K17" s="17">
+      <c r="H17" s="10"/>
+      <c r="I17" s="16">
+        <v>0</v>
+      </c>
+      <c r="J17" s="17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1743,14 +1785,14 @@
       <c r="E18" s="6"/>
       <c r="F18" s="10"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="18">
-        <v>0</v>
-      </c>
-      <c r="J18" s="19">
-        <v>0</v>
-      </c>
-      <c r="K18" s="17">
+      <c r="H18" s="10"/>
+      <c r="I18" s="16">
+        <v>0</v>
+      </c>
+      <c r="J18" s="17">
+        <v>0</v>
+      </c>
+      <c r="K18" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1762,14 +1804,14 @@
       <c r="E19" s="6"/>
       <c r="F19" s="10"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="18">
-        <v>0</v>
-      </c>
-      <c r="J19" s="19">
-        <v>0</v>
-      </c>
-      <c r="K19" s="17">
+      <c r="H19" s="10"/>
+      <c r="I19" s="16">
+        <v>0</v>
+      </c>
+      <c r="J19" s="17">
+        <v>0</v>
+      </c>
+      <c r="K19" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1781,14 +1823,14 @@
       <c r="E20" s="6"/>
       <c r="F20" s="10"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="18">
-        <v>0</v>
-      </c>
-      <c r="J20" s="19">
-        <v>0</v>
-      </c>
-      <c r="K20" s="17">
+      <c r="H20" s="10"/>
+      <c r="I20" s="16">
+        <v>0</v>
+      </c>
+      <c r="J20" s="17">
+        <v>0</v>
+      </c>
+      <c r="K20" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1800,14 +1842,14 @@
       <c r="E21" s="6"/>
       <c r="F21" s="10"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="18">
-        <v>0</v>
-      </c>
-      <c r="J21" s="19">
-        <v>0</v>
-      </c>
-      <c r="K21" s="17">
+      <c r="H21" s="10"/>
+      <c r="I21" s="16">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <v>0</v>
+      </c>
+      <c r="K21" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1819,14 +1861,14 @@
       <c r="E22" s="6"/>
       <c r="F22" s="10"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="18">
-        <v>0</v>
-      </c>
-      <c r="J22" s="19">
-        <v>0</v>
-      </c>
-      <c r="K22" s="17">
+      <c r="H22" s="10"/>
+      <c r="I22" s="16">
+        <v>0</v>
+      </c>
+      <c r="J22" s="17">
+        <v>0</v>
+      </c>
+      <c r="K22" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1838,14 +1880,14 @@
       <c r="E23" s="6"/>
       <c r="F23" s="10"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="18">
-        <v>0</v>
-      </c>
-      <c r="J23" s="19">
-        <v>0</v>
-      </c>
-      <c r="K23" s="17">
+      <c r="H23" s="10"/>
+      <c r="I23" s="16">
+        <v>0</v>
+      </c>
+      <c r="J23" s="17">
+        <v>0</v>
+      </c>
+      <c r="K23" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1857,14 +1899,14 @@
       <c r="E24" s="6"/>
       <c r="F24" s="10"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="18">
-        <v>0</v>
-      </c>
-      <c r="J24" s="19">
-        <v>0</v>
-      </c>
-      <c r="K24" s="17">
+      <c r="H24" s="10"/>
+      <c r="I24" s="16">
+        <v>0</v>
+      </c>
+      <c r="J24" s="17">
+        <v>0</v>
+      </c>
+      <c r="K24" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1876,14 +1918,14 @@
       <c r="E25" s="6"/>
       <c r="F25" s="10"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="18">
-        <v>0</v>
-      </c>
-      <c r="J25" s="19">
-        <v>0</v>
-      </c>
-      <c r="K25" s="17">
+      <c r="H25" s="10"/>
+      <c r="I25" s="16">
+        <v>0</v>
+      </c>
+      <c r="J25" s="17">
+        <v>0</v>
+      </c>
+      <c r="K25" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1895,14 +1937,14 @@
       <c r="E26" s="6"/>
       <c r="F26" s="10"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="18">
-        <v>0</v>
-      </c>
-      <c r="J26" s="19">
-        <v>0</v>
-      </c>
-      <c r="K26" s="17">
+      <c r="H26" s="10"/>
+      <c r="I26" s="16">
+        <v>0</v>
+      </c>
+      <c r="J26" s="17">
+        <v>0</v>
+      </c>
+      <c r="K26" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1914,14 +1956,14 @@
       <c r="E27" s="6"/>
       <c r="F27" s="10"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="18">
-        <v>0</v>
-      </c>
-      <c r="J27" s="19">
-        <v>0</v>
-      </c>
-      <c r="K27" s="17">
+      <c r="H27" s="10"/>
+      <c r="I27" s="16">
+        <v>0</v>
+      </c>
+      <c r="J27" s="17">
+        <v>0</v>
+      </c>
+      <c r="K27" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1933,14 +1975,14 @@
       <c r="E28" s="6"/>
       <c r="F28" s="10"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="18">
-        <v>0</v>
-      </c>
-      <c r="J28" s="19">
-        <v>0</v>
-      </c>
-      <c r="K28" s="17">
+      <c r="H28" s="10"/>
+      <c r="I28" s="16">
+        <v>0</v>
+      </c>
+      <c r="J28" s="17">
+        <v>0</v>
+      </c>
+      <c r="K28" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1952,14 +1994,14 @@
       <c r="E29" s="6"/>
       <c r="F29" s="10"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="18">
-        <v>0</v>
-      </c>
-      <c r="J29" s="19">
-        <v>0</v>
-      </c>
-      <c r="K29" s="17">
+      <c r="H29" s="10"/>
+      <c r="I29" s="16">
+        <v>0</v>
+      </c>
+      <c r="J29" s="17">
+        <v>0</v>
+      </c>
+      <c r="K29" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1969,27 +2011,27 @@
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="12"/>
+      <c r="F30" s="11"/>
       <c r="G30" s="8"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="20">
-        <v>0</v>
-      </c>
-      <c r="J30" s="19">
-        <v>0</v>
-      </c>
-      <c r="K30" s="17">
+      <c r="H30" s="11"/>
+      <c r="I30" s="18">
+        <v>0</v>
+      </c>
+      <c r="J30" s="17">
+        <v>0</v>
+      </c>
+      <c r="K30" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" ht="17.25" spans="10:11">
-      <c r="J31" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="K31" s="22">
+      <c r="J31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="K31" s="20">
         <f>SUM(K3:K30)</f>
-        <v>115.22</v>
+        <v>121.22</v>
       </c>
     </row>
     <row r="32" ht="15"/>

</xml_diff>

<commit_message>
changed current sense resistors to 700u
</commit_message>
<xml_diff>
--- a/documentation/rough-budget.xlsx
+++ b/documentation/rough-budget.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Component</t>
   </si>
@@ -97,6 +97,9 @@
     <t>CP2130</t>
   </si>
   <si>
+    <t>USB Uart Bridge</t>
+  </si>
+  <si>
     <t>Motor</t>
   </si>
   <si>
@@ -130,13 +133,16 @@
     <t>Sense Resistor</t>
   </si>
   <si>
-    <t>WSLF25121L000FEA</t>
-  </si>
-  <si>
-    <t>Vishay</t>
-  </si>
-  <si>
-    <t>1mΩ 6W</t>
+    <t xml:space="preserve">LRMAP3920B-R0007FT </t>
+  </si>
+  <si>
+    <t>IRC / TT Electronics</t>
+  </si>
+  <si>
+    <t>700uΩ 5W</t>
+  </si>
+  <si>
+    <t>Mouser | Farnell</t>
   </si>
   <si>
     <t>Current Amplifier</t>
@@ -149,6 +155,9 @@
   </si>
   <si>
     <t>Bidirectional, Zero Drift, Current Sense Amplifier High accuracy gain = 20</t>
+  </si>
+  <si>
+    <t>Bulk capacitors</t>
   </si>
   <si>
     <t>PCB</t>
@@ -171,11 +180,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="#,##0.00&quot;€&quot;;\-#,##0.00&quot;€&quot;"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="#,##0.00&quot;€&quot;;\-#,##0.00&quot;€&quot;"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -193,18 +202,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Georgia"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Georgia"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -223,6 +225,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Georgia"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Georgia"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Georgia"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -231,25 +255,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Georgia"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Georgia"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Georgia"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,15 +270,22 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Georgia"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="Georgia"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Georgia"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,30 +299,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Georgia"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Georgia"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Georgia"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Georgia"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -321,19 +314,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Georgia"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Georgia"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Georgia"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Georgia"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -364,43 +373,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,139 +547,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -713,6 +722,36 @@
       </top>
       <bottom style="thick">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -738,45 +777,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -787,15 +787,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -814,153 +805,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1343,7 +1352,7 @@
   <dimension ref="B1:K32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1416,7 +1425,7 @@
         <v>12.87</v>
       </c>
       <c r="K3" s="15">
-        <f>J3*I3</f>
+        <f t="shared" ref="K3:K7" si="0">J3*I3</f>
         <v>12.87</v>
       </c>
     </row>
@@ -1445,7 +1454,7 @@
         <v>3.05</v>
       </c>
       <c r="K4" s="15">
-        <f t="shared" ref="K4:K14" si="0">J4*I4</f>
+        <f t="shared" si="0"/>
         <v>12.2</v>
       </c>
     </row>
@@ -1513,159 +1522,151 @@
       <c r="B7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="17">
-        <v>45.46</v>
+        <v>0</v>
       </c>
       <c r="K7" s="15">
         <f t="shared" si="0"/>
-        <v>45.46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="2:11">
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>36</v>
+      <c r="H8" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="I8" s="16">
         <v>1</v>
       </c>
       <c r="J8" s="17">
-        <v>20</v>
+        <v>45.46</v>
       </c>
       <c r="K8" s="15">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f t="shared" ref="K8:K12" si="1">J8*I8</f>
+        <v>45.46</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="2:11">
       <c r="B9" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>19</v>
+      <c r="H9" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="I9" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="17">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="K9" s="15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" spans="2:11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" ht="30" spans="2:11">
       <c r="B10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="I10" s="16">
         <v>2</v>
       </c>
       <c r="J10" s="17">
-        <v>2.5</v>
+        <v>0.6</v>
       </c>
       <c r="K10" s="15">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>1.2</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:11">
       <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="16">
+        <v>2</v>
+      </c>
+      <c r="J11" s="17">
+        <v>2.5</v>
+      </c>
+      <c r="K11" s="15">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" spans="2:11">
+      <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="16">
-        <v>1</v>
-      </c>
-      <c r="J11" s="17">
-        <v>10</v>
-      </c>
-      <c r="K11" s="15">
-        <f>J11*I11</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" spans="2:11">
-      <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1673,24 +1674,36 @@
       <c r="G12" s="6"/>
       <c r="H12" s="10"/>
       <c r="I12" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J12" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="2:11">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="B13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="10"/>
+      <c r="G13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="I13" s="16">
         <v>0</v>
       </c>
@@ -1698,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="15">
-        <f t="shared" si="0"/>
+        <f>J13*I13</f>
         <v>0</v>
       </c>
     </row>
@@ -1717,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="15">
-        <f t="shared" si="0"/>
+        <f>J14*I14</f>
         <v>0</v>
       </c>
     </row>
@@ -1736,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="15">
-        <f t="shared" ref="K15:K30" si="1">J15*I15</f>
+        <f t="shared" ref="K15:K30" si="2">J15*I15</f>
         <v>0</v>
       </c>
     </row>
@@ -1755,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1774,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1793,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1812,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1831,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1850,7 +1863,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1869,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1888,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1907,7 +1920,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1926,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1945,7 +1958,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1964,7 +1977,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1983,7 +1996,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2002,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2021,17 +2034,17 @@
         <v>0</v>
       </c>
       <c r="K30" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" ht="17.25" spans="10:11">
       <c r="J31" s="19" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K31" s="20">
         <f>SUM(K3:K30)</f>
-        <v>121.22</v>
+        <v>115.42</v>
       </c>
     </row>
     <row r="32" ht="15"/>

</xml_diff>